<commit_message>
Requisito 9 - finalizado.
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="134">
   <si>
     <t xml:space="preserve">usuario_id</t>
   </si>
@@ -382,6 +382,9 @@
     <t xml:space="preserve">reprodution_date</t>
   </si>
   <si>
+    <t xml:space="preserve">207+3,69</t>
+  </si>
+  <si>
     <t xml:space="preserve">"2022-02-28 10:45:55"</t>
   </si>
   <si>
@@ -435,13 +438,12 @@
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -464,14 +466,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF111111"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -483,12 +477,6 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF111111"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
     </font>
@@ -561,7 +549,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="67">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -710,11 +698,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -754,7 +738,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -774,15 +758,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -798,11 +778,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -814,7 +790,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -822,7 +798,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -830,7 +806,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -922,10 +898,10 @@
   <dimension ref="A1:EY1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="1" sqref="B78:C91 F31"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.29"/>
@@ -939,6 +915,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="36.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="11" style="0" width="8.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="155" min="28" style="0" width="14.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -23377,8 +23354,8 @@
   </sheetPr>
   <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B78" activeCellId="0" sqref="B78:C91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C60" activeCellId="0" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23387,7 +23364,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="32" width="21.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="32" width="24.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="32" width="38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="32" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="32" width="18.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="32" width="9.14"/>
   </cols>
   <sheetData>
@@ -23416,7 +23393,7 @@
       <c r="D2" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="36" t="s">
         <v>95</v>
       </c>
       <c r="F2" s="0"/>
@@ -23424,19 +23401,19 @@
       <c r="H2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39" t="n">
+      <c r="A3" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="39" t="n">
+      <c r="C3" s="38" t="n">
         <v>82</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="41" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="0"/>
@@ -23444,19 +23421,19 @@
       <c r="H3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="n">
+      <c r="A4" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="39" t="n">
+      <c r="C4" s="38" t="n">
         <v>58</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="41" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="0"/>
@@ -23464,19 +23441,19 @@
       <c r="H4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39" t="n">
+      <c r="A5" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="39" t="n">
+      <c r="C5" s="38" t="n">
         <v>37</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="41" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="0"/>
@@ -23484,139 +23461,139 @@
       <c r="H5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="n">
+      <c r="A6" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="39" t="n">
+      <c r="C6" s="38" t="n">
         <v>46</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="41" t="s">
         <v>28</v>
       </c>
       <c r="F6" s="0"/>
       <c r="G6" s="0"/>
       <c r="H6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="n">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="38" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="39" t="n">
+      <c r="C7" s="38" t="n">
         <v>58</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="42" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="0"/>
       <c r="G7" s="0"/>
       <c r="H7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="n">
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="39" t="n">
+      <c r="C8" s="38" t="n">
         <v>19</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="42" t="s">
         <v>39</v>
       </c>
       <c r="F8" s="0"/>
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39" t="n">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="38" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="39" t="n">
+      <c r="C9" s="38" t="n">
         <v>26</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="42" t="s">
         <v>44</v>
       </c>
       <c r="F9" s="0"/>
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="n">
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="38" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="39" t="n">
+      <c r="C10" s="38" t="n">
         <v>85</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="42" t="s">
         <v>49</v>
       </c>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="n">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="38" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="39" t="n">
+      <c r="C11" s="38" t="n">
         <v>45</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="42" t="s">
         <v>53</v>
       </c>
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="n">
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="38" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="39" t="n">
+      <c r="C12" s="38" t="n">
         <v>58</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="42" t="s">
         <v>58</v>
       </c>
       <c r="F12" s="0"/>
@@ -23624,22 +23601,22 @@
       <c r="H12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="44"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="46" t="s">
+      <c r="A13" s="43"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="45" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="44"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="43"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="47" t="s">
         <v>101</v>
       </c>
       <c r="B15" s="36" t="s">
@@ -23650,46 +23627,46 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="50" t="n">
+      <c r="C16" s="49" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="50" t="n">
+      <c r="C17" s="49" t="n">
         <v>6.99</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="41" t="s">
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="51" t="n">
+      <c r="C18" s="50" t="n">
         <v>5.99</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="50" t="n">
+      <c r="C19" s="49" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -23728,17 +23705,17 @@
       <c r="G22" s="0"/>
       <c r="H22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="52" t="n">
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="52" t="n">
+      <c r="D23" s="51" t="n">
         <v>1</v>
       </c>
       <c r="E23" s="0"/>
@@ -23746,17 +23723,17 @@
       <c r="G23" s="0"/>
       <c r="H23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="52" t="n">
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="52" t="n">
+      <c r="D24" s="51" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="0"/>
@@ -23764,17 +23741,17 @@
       <c r="G24" s="0"/>
       <c r="H24" s="0"/>
     </row>
-    <row r="25" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="52" t="n">
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="51" t="n">
         <v>3</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C25" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="52" t="n">
+      <c r="D25" s="51" t="n">
         <v>2</v>
       </c>
       <c r="E25" s="0"/>
@@ -23782,17 +23759,17 @@
       <c r="G25" s="0"/>
       <c r="H25" s="0"/>
     </row>
-    <row r="26" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="52" t="n">
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="52" t="n">
+      <c r="D26" s="51" t="n">
         <v>3</v>
       </c>
       <c r="E26" s="0"/>
@@ -23800,17 +23777,17 @@
       <c r="G26" s="0"/>
       <c r="H26" s="0"/>
     </row>
-    <row r="27" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="52" t="n">
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="51" t="n">
         <v>5</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C27" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="52" t="n">
+      <c r="D27" s="51" t="n">
         <v>3</v>
       </c>
       <c r="E27" s="0"/>
@@ -23819,16 +23796,16 @@
       <c r="H27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="52" t="n">
+      <c r="A28" s="51" t="n">
         <v>6</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="52" t="n">
+      <c r="D28" s="51" t="n">
         <v>4</v>
       </c>
       <c r="E28" s="0"/>
@@ -23837,16 +23814,16 @@
       <c r="H28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="52" t="n">
+      <c r="A29" s="51" t="n">
         <v>7</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="52" t="n">
+      <c r="D29" s="51" t="n">
         <v>5</v>
       </c>
       <c r="E29" s="0"/>
@@ -23855,16 +23832,16 @@
       <c r="H29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="52" t="n">
+      <c r="A30" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="52" t="n">
+      <c r="D30" s="51" t="n">
         <v>6</v>
       </c>
       <c r="E30" s="0"/>
@@ -23873,13 +23850,13 @@
       <c r="H30" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="B33" s="47"/>
+      <c r="B33" s="46"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="48" t="s">
+      <c r="A34" s="47" t="s">
         <v>106</v>
       </c>
       <c r="B34" s="36" t="s">
@@ -23887,50 +23864,50 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="52" t="n">
+      <c r="A35" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="B35" s="52" t="s">
+      <c r="B35" s="51" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="52" t="n">
+      <c r="A36" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="51" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="52" t="n">
+      <c r="A37" s="51" t="n">
         <v>3</v>
       </c>
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="51" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="52" t="n">
+      <c r="A38" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="51" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="52" t="n">
+      <c r="A39" s="51" t="n">
         <v>5</v>
       </c>
-      <c r="B39" s="52" t="s">
+      <c r="B39" s="51" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="52" t="n">
+      <c r="A40" s="51" t="n">
         <v>6</v>
       </c>
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="51" t="s">
         <v>45</v>
       </c>
     </row>
@@ -23955,7 +23932,7 @@
       <c r="H42" s="33"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="52" t="s">
         <v>110</v>
       </c>
       <c r="B43" s="35" t="s">
@@ -23964,10 +23941,10 @@
       <c r="C43" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="D43" s="54" t="s">
+      <c r="D43" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="40" t="s">
+      <c r="E43" s="39" t="s">
         <v>111</v>
       </c>
       <c r="F43" s="0"/>
@@ -23975,19 +23952,19 @@
       <c r="H43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="39" t="n">
+      <c r="A44" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="B44" s="55" t="s">
+      <c r="B44" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="39" t="n">
+      <c r="C44" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="D44" s="52" t="n">
+      <c r="D44" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="E44" s="40" t="n">
+      <c r="E44" s="39" t="n">
         <v>279</v>
       </c>
       <c r="F44" s="0"/>
@@ -23995,19 +23972,19 @@
       <c r="H44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="39" t="n">
+      <c r="A45" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="B45" s="55" t="s">
+      <c r="B45" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="40" t="n">
+      <c r="C45" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="D45" s="52" t="n">
+      <c r="D45" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="E45" s="40" t="n">
+      <c r="E45" s="39" t="n">
         <v>369</v>
       </c>
       <c r="F45" s="0"/>
@@ -24015,159 +23992,159 @@
       <c r="H45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="39" t="n">
+      <c r="A46" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="B46" s="55" t="s">
+      <c r="B46" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="C46" s="40" t="n">
+      <c r="C46" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="D46" s="52" t="n">
+      <c r="D46" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="E46" s="40" t="n">
+      <c r="E46" s="39" t="n">
         <v>116</v>
       </c>
       <c r="F46" s="0"/>
       <c r="G46" s="0"/>
       <c r="H46" s="0"/>
     </row>
-    <row r="47" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="39" t="n">
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="39" t="n">
+      <c r="C47" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="D47" s="52" t="n">
+      <c r="D47" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="E47" s="52" t="n">
+      <c r="E47" s="51" t="n">
         <v>203</v>
       </c>
       <c r="F47" s="0"/>
       <c r="G47" s="0"/>
       <c r="H47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="39" t="n">
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="38" t="n">
         <v>5</v>
       </c>
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="C48" s="39" t="n">
+      <c r="C48" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="D48" s="52" t="n">
+      <c r="D48" s="51" t="n">
         <v>3</v>
       </c>
-      <c r="E48" s="52" t="n">
+      <c r="E48" s="51" t="n">
         <v>152</v>
       </c>
       <c r="F48" s="0"/>
       <c r="G48" s="0"/>
       <c r="H48" s="0"/>
     </row>
-    <row r="49" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="39" t="n">
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="39" t="n">
+      <c r="C49" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="D49" s="52" t="n">
+      <c r="D49" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E49" s="52" t="n">
+      <c r="E49" s="51" t="n">
         <v>105</v>
       </c>
       <c r="F49" s="0"/>
       <c r="G49" s="0"/>
       <c r="H49" s="0"/>
     </row>
-    <row r="50" customFormat="false" ht="28.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="39" t="n">
+    <row r="50" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="38" t="n">
         <v>7</v>
       </c>
-      <c r="B50" s="56" t="s">
+      <c r="B50" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="C50" s="39" t="n">
+      <c r="C50" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="D50" s="52" t="n">
+      <c r="D50" s="51" t="n">
         <v>5</v>
       </c>
-      <c r="E50" s="52" t="n">
+      <c r="E50" s="51" t="n">
         <v>207</v>
       </c>
       <c r="F50" s="0"/>
       <c r="G50" s="0"/>
       <c r="H50" s="0"/>
     </row>
-    <row r="51" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="39" t="n">
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="38" t="n">
         <v>8</v>
       </c>
-      <c r="B51" s="56" t="s">
+      <c r="B51" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="C51" s="39" t="n">
+      <c r="C51" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="D51" s="52" t="n">
+      <c r="D51" s="51" t="n">
         <v>6</v>
       </c>
-      <c r="E51" s="52" t="n">
+      <c r="E51" s="51" t="n">
         <v>267</v>
       </c>
       <c r="F51" s="0"/>
       <c r="G51" s="0"/>
       <c r="H51" s="0"/>
     </row>
-    <row r="52" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="40" t="n">
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="39" t="n">
         <v>9</v>
       </c>
-      <c r="B52" s="56" t="s">
+      <c r="B52" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="39" t="n">
+      <c r="C52" s="38" t="n">
         <v>5</v>
       </c>
-      <c r="D52" s="52" t="n">
+      <c r="D52" s="51" t="n">
         <v>7</v>
       </c>
-      <c r="E52" s="52" t="n">
+      <c r="E52" s="51" t="n">
         <v>244</v>
       </c>
       <c r="F52" s="0"/>
       <c r="G52" s="0"/>
       <c r="H52" s="0"/>
     </row>
-    <row r="53" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="40" t="n">
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="39" t="n">
         <v>10</v>
       </c>
-      <c r="B53" s="56" t="s">
+      <c r="B53" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="39" t="n">
+      <c r="C53" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="D53" s="52" t="n">
+      <c r="D53" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E53" s="52" t="n">
+      <c r="E53" s="51" t="n">
         <v>100</v>
       </c>
       <c r="F53" s="0"/>
@@ -24189,35 +24166,37 @@
       <c r="H56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="57" t="s">
+      <c r="A57" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="B57" s="58" t="s">
+      <c r="B57" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="C57" s="59" t="s">
+      <c r="C57" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="D57" s="60" t="s">
+      <c r="D57" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="E57" s="0"/>
+      <c r="E57" s="0" t="s">
+        <v>119</v>
+      </c>
       <c r="F57" s="0"/>
       <c r="G57" s="0"/>
       <c r="H57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="40" t="n">
+      <c r="A58" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="B58" s="61" t="n">
+      <c r="B58" s="58" t="n">
         <v>1</v>
       </c>
-      <c r="C58" s="61" t="n">
-        <v>7</v>
-      </c>
-      <c r="D58" s="62" t="s">
-        <v>119</v>
+      <c r="C58" s="58" t="n">
+        <v>8</v>
+      </c>
+      <c r="D58" s="59" t="s">
+        <v>120</v>
       </c>
       <c r="E58" s="0"/>
       <c r="F58" s="0"/>
@@ -24225,17 +24204,17 @@
       <c r="H58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="40" t="n">
+      <c r="A59" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="B59" s="61" t="n">
+      <c r="B59" s="58" t="n">
         <v>1</v>
       </c>
-      <c r="C59" s="61" t="n">
+      <c r="C59" s="58" t="n">
         <v>2</v>
       </c>
-      <c r="D59" s="62" t="s">
-        <v>120</v>
+      <c r="D59" s="59" t="s">
+        <v>121</v>
       </c>
       <c r="E59" s="0"/>
       <c r="F59" s="0"/>
@@ -24243,17 +24222,17 @@
       <c r="H59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="40" t="n">
+      <c r="A60" s="39" t="n">
         <v>3</v>
       </c>
-      <c r="B60" s="61" t="n">
+      <c r="B60" s="58" t="n">
         <v>1</v>
       </c>
-      <c r="C60" s="61" t="n">
+      <c r="C60" s="58" t="n">
         <v>10</v>
       </c>
-      <c r="D60" s="62" t="s">
-        <v>121</v>
+      <c r="D60" s="59" t="s">
+        <v>122</v>
       </c>
       <c r="E60" s="0"/>
       <c r="F60" s="0"/>
@@ -24261,17 +24240,17 @@
       <c r="H60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="40" t="n">
+      <c r="A61" s="39" t="n">
         <v>4</v>
       </c>
-      <c r="B61" s="61" t="n">
+      <c r="B61" s="58" t="n">
         <v>2</v>
       </c>
-      <c r="C61" s="61" t="n">
+      <c r="C61" s="58" t="n">
         <v>10</v>
       </c>
-      <c r="D61" s="56" t="s">
-        <v>122</v>
+      <c r="D61" s="54" t="s">
+        <v>123</v>
       </c>
       <c r="E61" s="0"/>
       <c r="F61" s="0"/>
@@ -24279,17 +24258,17 @@
       <c r="H61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="40" t="n">
+      <c r="A62" s="39" t="n">
         <v>5</v>
       </c>
-      <c r="B62" s="61" t="n">
+      <c r="B62" s="58" t="n">
         <v>2</v>
       </c>
-      <c r="C62" s="61" t="n">
+      <c r="C62" s="58" t="n">
         <v>7</v>
       </c>
-      <c r="D62" s="56" t="s">
-        <v>123</v>
+      <c r="D62" s="54" t="s">
+        <v>124</v>
       </c>
       <c r="E62" s="0"/>
       <c r="F62" s="0"/>
@@ -24297,17 +24276,17 @@
       <c r="H62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="40" t="n">
+      <c r="A63" s="39" t="n">
         <v>6</v>
       </c>
-      <c r="B63" s="61" t="n">
+      <c r="B63" s="58" t="n">
         <v>3</v>
       </c>
-      <c r="C63" s="61" t="n">
+      <c r="C63" s="58" t="n">
         <v>10</v>
       </c>
-      <c r="D63" s="56" t="s">
-        <v>124</v>
+      <c r="D63" s="54" t="s">
+        <v>125</v>
       </c>
       <c r="E63" s="0"/>
       <c r="F63" s="0"/>
@@ -24315,17 +24294,17 @@
       <c r="H63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="40" t="n">
+      <c r="A64" s="39" t="n">
         <v>7</v>
       </c>
-      <c r="B64" s="61" t="n">
+      <c r="B64" s="58" t="n">
         <v>3</v>
       </c>
-      <c r="C64" s="61" t="n">
+      <c r="C64" s="58" t="n">
         <v>2</v>
       </c>
-      <c r="D64" s="56" t="s">
-        <v>125</v>
+      <c r="D64" s="54" t="s">
+        <v>126</v>
       </c>
       <c r="E64" s="0"/>
       <c r="F64" s="0"/>
@@ -24333,17 +24312,17 @@
       <c r="H64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="40" t="n">
+      <c r="A65" s="39" t="n">
         <v>8</v>
       </c>
-      <c r="B65" s="61" t="n">
+      <c r="B65" s="58" t="n">
         <v>4</v>
       </c>
-      <c r="C65" s="61" t="n">
+      <c r="C65" s="58" t="n">
         <v>8</v>
       </c>
-      <c r="D65" s="63" t="s">
-        <v>126</v>
+      <c r="D65" s="60" t="s">
+        <v>127</v>
       </c>
       <c r="E65" s="0"/>
       <c r="F65" s="0"/>
@@ -24351,17 +24330,17 @@
       <c r="H65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="40" t="n">
+      <c r="A66" s="39" t="n">
         <v>9</v>
       </c>
-      <c r="B66" s="61" t="n">
+      <c r="B66" s="58" t="n">
         <v>5</v>
       </c>
-      <c r="C66" s="61" t="n">
+      <c r="C66" s="58" t="n">
         <v>8</v>
       </c>
-      <c r="D66" s="56" t="s">
-        <v>127</v>
+      <c r="D66" s="54" t="s">
+        <v>128</v>
       </c>
       <c r="E66" s="0"/>
       <c r="F66" s="0"/>
@@ -24369,17 +24348,17 @@
       <c r="H66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="40" t="n">
+      <c r="A67" s="39" t="n">
         <v>10</v>
       </c>
-      <c r="B67" s="61" t="n">
+      <c r="B67" s="58" t="n">
         <v>5</v>
       </c>
-      <c r="C67" s="61" t="n">
+      <c r="C67" s="58" t="n">
         <v>5</v>
       </c>
-      <c r="D67" s="56" t="s">
-        <v>128</v>
+      <c r="D67" s="54" t="s">
+        <v>129</v>
       </c>
       <c r="E67" s="0"/>
       <c r="F67" s="0"/>
@@ -24387,31 +24366,31 @@
       <c r="H67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="40" t="n">
+      <c r="A68" s="39" t="n">
         <v>11</v>
       </c>
-      <c r="B68" s="61" t="n">
+      <c r="B68" s="58" t="n">
         <v>6</v>
       </c>
-      <c r="C68" s="61" t="n">
+      <c r="C68" s="58" t="n">
         <v>7</v>
       </c>
-      <c r="D68" s="56" t="s">
-        <v>129</v>
+      <c r="D68" s="54" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="40" t="n">
+      <c r="A69" s="39" t="n">
         <v>12</v>
       </c>
-      <c r="B69" s="61" t="n">
+      <c r="B69" s="58" t="n">
         <v>6</v>
       </c>
-      <c r="C69" s="61" t="n">
+      <c r="C69" s="58" t="n">
         <v>1</v>
       </c>
-      <c r="D69" s="56" t="s">
-        <v>130</v>
+      <c r="D69" s="54" t="s">
+        <v>131</v>
       </c>
       <c r="E69" s="0"/>
       <c r="F69" s="0"/>
@@ -24419,16 +24398,16 @@
       <c r="H69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="40" t="n">
+      <c r="A70" s="39" t="n">
         <v>13</v>
       </c>
-      <c r="B70" s="61" t="n">
+      <c r="B70" s="58" t="n">
         <v>7</v>
       </c>
-      <c r="C70" s="61" t="n">
+      <c r="C70" s="58" t="n">
         <v>4</v>
       </c>
-      <c r="D70" s="56" t="s">
+      <c r="D70" s="54" t="s">
         <v>43</v>
       </c>
       <c r="E70" s="0"/>
@@ -24437,16 +24416,16 @@
       <c r="H70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="40" t="n">
+      <c r="A71" s="39" t="n">
         <v>14</v>
       </c>
-      <c r="B71" s="61" t="n">
+      <c r="B71" s="58" t="n">
         <v>8</v>
       </c>
-      <c r="C71" s="61" t="n">
+      <c r="C71" s="58" t="n">
         <v>4</v>
       </c>
-      <c r="D71" s="56" t="s">
+      <c r="D71" s="54" t="s">
         <v>47</v>
       </c>
       <c r="E71" s="0"/>
@@ -24455,16 +24434,16 @@
       <c r="H71" s="0"/>
     </row>
     <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="40" t="n">
+      <c r="A72" s="39" t="n">
         <v>15</v>
       </c>
-      <c r="B72" s="61" t="n">
+      <c r="B72" s="58" t="n">
         <v>9</v>
       </c>
-      <c r="C72" s="61" t="n">
+      <c r="C72" s="58" t="n">
         <v>9</v>
       </c>
-      <c r="D72" s="56" t="s">
+      <c r="D72" s="54" t="s">
         <v>52</v>
       </c>
       <c r="E72" s="0"/>
@@ -24473,16 +24452,16 @@
       <c r="H72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="40" t="n">
+      <c r="A73" s="39" t="n">
         <v>16</v>
       </c>
-      <c r="B73" s="61" t="n">
+      <c r="B73" s="58" t="n">
         <v>10</v>
       </c>
-      <c r="C73" s="61" t="n">
-        <v>2</v>
-      </c>
-      <c r="D73" s="56" t="s">
+      <c r="C73" s="58" t="n">
+        <v>3</v>
+      </c>
+      <c r="D73" s="54" t="s">
         <v>57</v>
       </c>
       <c r="E73" s="0"/>
@@ -24490,9 +24469,11 @@
       <c r="G73" s="0"/>
       <c r="H73" s="0"/>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0"/>
-      <c r="B74" s="0"/>
+      <c r="B74" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="C74" s="0"/>
       <c r="D74" s="0"/>
       <c r="E74" s="0"/>
@@ -24501,10 +24482,10 @@
       <c r="H74" s="0"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="64" t="s">
-        <v>131</v>
-      </c>
-      <c r="B76" s="64"/>
+      <c r="A76" s="61" t="s">
+        <v>132</v>
+      </c>
+      <c r="B76" s="61"/>
       <c r="C76" s="0"/>
       <c r="D76" s="0" t="s">
         <v>116</v>
@@ -24515,13 +24496,13 @@
       <c r="H76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="B77" s="66" t="s">
+      <c r="A77" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="B77" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="C77" s="67" t="s">
+      <c r="C77" s="64" t="s">
         <v>106</v>
       </c>
       <c r="D77" s="0"/>
@@ -24534,10 +24515,10 @@
       <c r="A78" s="32" t="n">
         <v>1</v>
       </c>
-      <c r="B78" s="61" t="n">
+      <c r="B78" s="58" t="n">
         <v>1</v>
       </c>
-      <c r="C78" s="68" t="n">
+      <c r="C78" s="65" t="n">
         <v>1</v>
       </c>
       <c r="D78" s="0"/>
@@ -24550,10 +24531,10 @@
       <c r="A79" s="32" t="n">
         <v>2</v>
       </c>
-      <c r="B79" s="61" t="n">
+      <c r="B79" s="58" t="n">
         <v>1</v>
       </c>
-      <c r="C79" s="61" t="n">
+      <c r="C79" s="58" t="n">
         <v>2</v>
       </c>
       <c r="D79" s="0"/>
@@ -24566,10 +24547,10 @@
       <c r="A80" s="32" t="n">
         <v>3</v>
       </c>
-      <c r="B80" s="61" t="n">
+      <c r="B80" s="58" t="n">
         <v>1</v>
       </c>
-      <c r="C80" s="61" t="n">
+      <c r="C80" s="58" t="n">
         <v>3</v>
       </c>
       <c r="D80" s="0"/>
@@ -24582,10 +24563,10 @@
       <c r="A81" s="32" t="n">
         <v>4</v>
       </c>
-      <c r="B81" s="61" t="n">
+      <c r="B81" s="58" t="n">
         <v>2</v>
       </c>
-      <c r="C81" s="61" t="n">
+      <c r="C81" s="58" t="n">
         <v>1</v>
       </c>
       <c r="D81" s="0"/>
@@ -24598,10 +24579,10 @@
       <c r="A82" s="32" t="n">
         <v>5</v>
       </c>
-      <c r="B82" s="61" t="n">
+      <c r="B82" s="58" t="n">
         <v>2</v>
       </c>
-      <c r="C82" s="61" t="n">
+      <c r="C82" s="58" t="n">
         <v>3</v>
       </c>
       <c r="D82" s="0"/>
@@ -24614,10 +24595,10 @@
       <c r="A83" s="32" t="n">
         <v>6</v>
       </c>
-      <c r="B83" s="61" t="n">
+      <c r="B83" s="58" t="n">
         <v>3</v>
       </c>
-      <c r="C83" s="61" t="n">
+      <c r="C83" s="58" t="n">
         <v>2</v>
       </c>
       <c r="D83" s="0"/>
@@ -24630,10 +24611,10 @@
       <c r="A84" s="32" t="n">
         <v>7</v>
       </c>
-      <c r="B84" s="61" t="n">
+      <c r="B84" s="58" t="n">
         <v>4</v>
       </c>
-      <c r="C84" s="61" t="n">
+      <c r="C84" s="58" t="n">
         <v>4</v>
       </c>
       <c r="D84" s="0"/>
@@ -24646,10 +24627,10 @@
       <c r="A85" s="32" t="n">
         <v>8</v>
       </c>
-      <c r="B85" s="61" t="n">
+      <c r="B85" s="58" t="n">
         <v>5</v>
       </c>
-      <c r="C85" s="61" t="n">
+      <c r="C85" s="58" t="n">
         <v>5</v>
       </c>
       <c r="D85" s="0"/>
@@ -24662,10 +24643,10 @@
       <c r="A86" s="32" t="n">
         <v>9</v>
       </c>
-      <c r="B86" s="61" t="n">
+      <c r="B86" s="58" t="n">
         <v>5</v>
       </c>
-      <c r="C86" s="61" t="n">
+      <c r="C86" s="58" t="n">
         <v>6</v>
       </c>
       <c r="D86" s="0"/>
@@ -24678,10 +24659,10 @@
       <c r="A87" s="32" t="n">
         <v>10</v>
       </c>
-      <c r="B87" s="61" t="n">
+      <c r="B87" s="58" t="n">
         <v>6</v>
       </c>
-      <c r="C87" s="61" t="n">
+      <c r="C87" s="58" t="n">
         <v>6</v>
       </c>
       <c r="D87" s="0"/>
@@ -24694,10 +24675,10 @@
       <c r="A88" s="32" t="n">
         <v>11</v>
       </c>
-      <c r="B88" s="61" t="n">
+      <c r="B88" s="58" t="n">
         <v>6</v>
       </c>
-      <c r="C88" s="61" t="n">
+      <c r="C88" s="58" t="n">
         <v>1</v>
       </c>
       <c r="D88" s="0"/>
@@ -24710,10 +24691,10 @@
       <c r="A89" s="32" t="n">
         <v>12</v>
       </c>
-      <c r="B89" s="61" t="n">
+      <c r="B89" s="58" t="n">
         <v>7</v>
       </c>
-      <c r="C89" s="61" t="n">
+      <c r="C89" s="58" t="n">
         <v>6</v>
       </c>
       <c r="D89" s="0"/>
@@ -24726,10 +24707,10 @@
       <c r="A90" s="32" t="n">
         <v>13</v>
       </c>
-      <c r="B90" s="61" t="n">
+      <c r="B90" s="58" t="n">
         <v>9</v>
       </c>
-      <c r="C90" s="61" t="n">
+      <c r="C90" s="58" t="n">
         <v>3</v>
       </c>
       <c r="D90" s="0"/>
@@ -24742,10 +24723,10 @@
       <c r="A91" s="32" t="n">
         <v>14</v>
       </c>
-      <c r="B91" s="61" t="n">
+      <c r="B91" s="58" t="n">
         <v>10</v>
       </c>
-      <c r="C91" s="61" t="n">
+      <c r="C91" s="58" t="n">
         <v>2</v>
       </c>
       <c r="D91" s="0"/>
@@ -24758,7 +24739,7 @@
       <c r="A92" s="32" t="n">
         <v>15</v>
       </c>
-      <c r="B92" s="69"/>
+      <c r="B92" s="66"/>
       <c r="C92" s="0"/>
       <c r="D92" s="0"/>
       <c r="E92" s="0"/>
@@ -24767,7 +24748,7 @@
       <c r="H92" s="0"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="69"/>
+      <c r="A93" s="66"/>
       <c r="B93" s="0"/>
       <c r="C93" s="0"/>
       <c r="D93" s="0"/>

</xml_diff>